<commit_message>
Actualizacion del data set
</commit_message>
<xml_diff>
--- a/Data/DatasetRelaciones.xlsx
+++ b/Data/DatasetRelaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferof\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE48E92B-27A8-4DB0-8CD0-3D1FB85404C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A65C9C-A06A-44A7-83E8-2D9459470F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5748" yWindow="660" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="150">
   <si>
     <t>Origen</t>
   </si>
@@ -470,9 +470,6 @@
     <t xml:space="preserve">Lorena Coghi </t>
   </si>
   <si>
-    <t xml:space="preserve">Mario Ordoñez Ramirez </t>
-  </si>
-  <si>
     <t>Adolfo Lazo</t>
   </si>
   <si>
@@ -480,6 +477,15 @@
   </si>
   <si>
     <t>Marcelo Torres</t>
+  </si>
+  <si>
+    <t>Mario Ordoñez</t>
+  </si>
+  <si>
+    <t>Kevin Jimenez</t>
+  </si>
+  <si>
+    <t>Glenda Correa</t>
   </si>
 </sst>
 </file>
@@ -679,9 +685,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -715,19 +718,22 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -782,11 +788,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B132" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="3" tableBorderDxfId="4">
-  <autoFilter ref="A1:B132" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B134" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+  <autoFilter ref="A1:B134" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7F64902A-E321-4079-A813-031231175E65}" name="Origen" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1452E443-F698-4C0B-99ED-CB17F3F96C12}" name="Destino" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7F64902A-E321-4079-A813-031231175E65}" name="Origen" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1452E443-F698-4C0B-99ED-CB17F3F96C12}" name="Destino" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1079,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2121,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -2129,7 +2135,7 @@
         <v>142</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2137,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -2145,7 +2151,23 @@
         <v>2</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="9" t="s">
         <v>147</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva actualizacion del dataset y añadido de bash para cerrar puertos
</commit_message>
<xml_diff>
--- a/Data/DatasetRelaciones.xlsx
+++ b/Data/DatasetRelaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferof\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79376FB8-394D-4D4B-A499-9DA2C9A72A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD87E3-E3AF-4AB9-8983-5DAAB4143479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="149">
   <si>
     <t>Origen</t>
   </si>
@@ -794,8 +794,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B134" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
-  <autoFilter ref="A1:B134" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B136" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+  <autoFilter ref="A1:B136" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7F64902A-E321-4079-A813-031231175E65}" name="Origen" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{1452E443-F698-4C0B-99ED-CB17F3F96C12}" name="Destino" dataDxfId="0"/>
@@ -1091,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2177,6 +2177,18 @@
         <v>148</v>
       </c>
     </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="9"/>
+      <c r="B136" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Acrualizacion del dataset 5
</commit_message>
<xml_diff>
--- a/Data/DatasetRelaciones.xlsx
+++ b/Data/DatasetRelaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferof\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD87E3-E3AF-4AB9-8983-5DAAB4143479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875D41E-62C7-4950-AD38-46CA7CABDED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="145">
   <si>
     <t>Origen</t>
   </si>
@@ -107,18 +107,12 @@
     <t>Raúl Borja</t>
   </si>
   <si>
-    <t>Jose Zambrano</t>
-  </si>
-  <si>
     <t>Antonio Muñoz</t>
   </si>
   <si>
     <t>Christian Calderón</t>
   </si>
   <si>
-    <t>Enrique Garcia</t>
-  </si>
-  <si>
     <t>Israel Ortega</t>
   </si>
   <si>
@@ -167,12 +161,6 @@
     <t>James Santana</t>
   </si>
   <si>
-    <t>Jose holguin</t>
-  </si>
-  <si>
-    <t>Enrique Garcia Valdez</t>
-  </si>
-  <si>
     <t>Paula Valdez Peralta</t>
   </si>
   <si>
@@ -434,9 +422,6 @@
     <t>Mattews Montes</t>
   </si>
   <si>
-    <t>Henry Salvatierra</t>
-  </si>
-  <si>
     <t>Jeremi Silva</t>
   </si>
   <si>
@@ -461,12 +446,6 @@
     <t>Juleysi Reyes</t>
   </si>
   <si>
-    <t xml:space="preserve">Ángeles correa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorena Coghi </t>
-  </si>
-  <si>
     <t>Adolfo Lazo</t>
   </si>
   <si>
@@ -483,6 +462,15 @@
   </si>
   <si>
     <t>Glenda Correa</t>
+  </si>
+  <si>
+    <t>Jose Holguin</t>
+  </si>
+  <si>
+    <t>Lorena Coghi</t>
+  </si>
+  <si>
+    <t>Ángeles Correa</t>
   </si>
 </sst>
 </file>
@@ -648,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,9 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -724,6 +709,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -737,13 +729,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -794,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B136" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
-  <autoFilter ref="A1:B136" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}" name="Table1" displayName="Table1" ref="A1:B134" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:B134" xr:uid="{E3D54304-F01D-4FF8-B918-9B246E1C2D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7F64902A-E321-4079-A813-031231175E65}" name="Origen" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{1452E443-F698-4C0B-99ED-CB17F3F96C12}" name="Destino" dataDxfId="0"/>
@@ -1093,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,7 +1170,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
@@ -1193,7 +1178,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -1248,7 +1233,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1256,91 +1241,91 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
+      <c r="B22" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1353,138 +1338,138 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1492,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1500,47 +1485,47 @@
         <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1548,216 +1533,216 @@
         <v>2</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E68" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="E68" s="12"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1765,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1773,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1781,7 +1766,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1789,7 +1774,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1797,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1805,31 +1790,31 @@
         <v>2</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1837,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1845,15 +1830,15 @@
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1861,7 +1846,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1869,39 +1854,39 @@
         <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1909,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -1917,39 +1902,39 @@
         <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1957,7 +1942,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -1965,200 +1950,200 @@
         <v>2</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B122" s="1" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C128" s="10"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="11" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C128" s="10"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B129" s="11" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="11" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="12" t="s">
+      <c r="A131" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="9" t="s">
+      <c r="A132" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -2166,24 +2151,20 @@
         <v>2</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="A135" s="9"/>
+      <c r="B135" s="3"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="9"/>

</xml_diff>